<commit_message>
assets/excel-files replaced with assets/workbooks
</commit_message>
<xml_diff>
--- a/assets/workbooks/Annuity-Factors-Calculator-v.02.xlsx
+++ b/assets/workbooks/Annuity-Factors-Calculator-v.02.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyau\Documents\ActuarialAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B49122-4E40-4F8C-AC28-A3897D28D128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B872739-05B6-4505-B643-7D70AA69429F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF301219-F2C0-4040-9DBA-23E8E2F8303E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FF301219-F2C0-4040-9DBA-23E8E2F8303E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Annuity factor" sheetId="3" r:id="rId1"/>
-    <sheet name="Annuitants" sheetId="1" r:id="rId2"/>
-    <sheet name="Settings" sheetId="5" r:id="rId3"/>
-    <sheet name="Lists" sheetId="4" r:id="rId4"/>
-    <sheet name="Transfo" sheetId="2" r:id="rId5"/>
+    <sheet name="User guide" sheetId="6" r:id="rId1"/>
+    <sheet name="Annuity factor" sheetId="3" r:id="rId2"/>
+    <sheet name="Annuitants" sheetId="1" r:id="rId3"/>
+    <sheet name="Settings" sheetId="5" r:id="rId4"/>
+    <sheet name="Lists" sheetId="4" r:id="rId5"/>
+    <sheet name="Transfo" sheetId="2" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="_cia_indexation_available">Transfo!$B$26</definedName>
@@ -115,14 +116,14 @@
     <definedName name="_listQxScale_US">Lists!$O$3:$O$10</definedName>
     <definedName name="_listQxTable">IF(_s_country="United States",_listQxTable_US,_listQxTable_CAN)</definedName>
     <definedName name="_listQxTable_CAN">Lists!$H$3:$H$21</definedName>
-    <definedName name="_listQxTable_US">Lists!$L$3:$L$16</definedName>
+    <definedName name="_listQxTable_US">Lists!$L$3:$L$51</definedName>
     <definedName name="_listReversion">Lists!$E$3:$E$8</definedName>
     <definedName name="_listSex">Lists!$D$3:$D$4</definedName>
     <definedName name="_r_annuityFactor">'Annuity factor'!$B$27</definedName>
-    <definedName name="_s_country">Settings!$B$13</definedName>
+    <definedName name="_s_country">Settings!$B$15</definedName>
     <definedName name="_s_error1">Settings!$B$5</definedName>
-    <definedName name="_s_error2">Settings!$B$12</definedName>
-    <definedName name="_settings_invalid">Settings!$B$16</definedName>
+    <definedName name="_s_error2">Settings!$B$14</definedName>
+    <definedName name="_settings_invalid">Settings!$B$18</definedName>
     <definedName name="_show_results">Transfo!$B$32</definedName>
     <definedName name="_t_age1">Transfo!$C$8</definedName>
     <definedName name="_t_age2">Transfo!$C$9</definedName>
@@ -171,12 +172,12 @@
     <definedName name="_t_sex2_temp">Transfo!$C$6</definedName>
     <definedName name="_t_today">Transfo!$B$55</definedName>
     <definedName name="_tabCountry">Lists!$A$3:$B$4</definedName>
-    <definedName name="_tabFormat">Settings!$D$6:$E$16</definedName>
+    <definedName name="_tabFormat">Settings!$D$6:$E$18</definedName>
     <definedName name="_tabFormatOffset">Settings!$C$6</definedName>
     <definedName name="_tabPersons">Annuitants!$A:$I</definedName>
     <definedName name="_tabQxTable">IF(_s_country="United States",_tabQxTable_US,_tabQxTable_CAN)</definedName>
     <definedName name="_tabQxTable_CAN">Lists!$H$4:$J$21</definedName>
-    <definedName name="_tabQxTable_US">Lists!$L$4:$N$16</definedName>
+    <definedName name="_tabQxTable_US">Lists!$L$4:$N$51</definedName>
     <definedName name="_z_idMax">MAX(Annuitants!$A:$A)</definedName>
     <definedName name="_z_idMin">MIN(Annuitants!$A:$A)</definedName>
     <definedName name="_z_tabQxTable">IF(OR(_t_country="CAN",_t_cia_interest_show),_tabQxTable_CAN,_tabQxTable_US)</definedName>
@@ -260,7 +261,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="289">
   <si>
     <t>ID</t>
   </si>
@@ -785,21 +786,9 @@
     <t>RP-2014 Rates-Employee</t>
   </si>
   <si>
-    <t>RP-2014 Rates-Employee-Blue Collar</t>
-  </si>
-  <si>
-    <t>RP-2014 Rates-Employee-White Collar</t>
-  </si>
-  <si>
     <t>RP-2014 Rates-Healthy annuitant</t>
   </si>
   <si>
-    <t>RP-2014 Rates-Healthy annuitant-Blue Collar</t>
-  </si>
-  <si>
-    <t>RP-2014 Rates-Healthy annuitant-White Collar</t>
-  </si>
-  <si>
     <t>RP-2014 Rates-Disabled annuitant</t>
   </si>
   <si>
@@ -815,18 +804,6 @@
     <t>RP2014E_BOTTOM</t>
   </si>
   <si>
-    <t>RP-2014 Rates-Employee-Top quartile (salary)</t>
-  </si>
-  <si>
-    <t>RP-2014 Rates-Employee-Bottom quartile (salary)</t>
-  </si>
-  <si>
-    <t>RP-2014 Rates-Healthy annuitant-Top quartile (benefit)</t>
-  </si>
-  <si>
-    <t>RP-2014 Rates-Healthy annuitant-Bottom quartile (benefit)</t>
-  </si>
-  <si>
     <t>Period Life Table, 2019 (population mortality)</t>
   </si>
   <si>
@@ -843,33 +820,6 @@
   </si>
   <si>
     <t>USA</t>
-  </si>
-  <si>
-    <t>Life Tables, Canada population, 2017/2019</t>
-  </si>
-  <si>
-    <t>Life Tables, Canada population, 2016/2018</t>
-  </si>
-  <si>
-    <t>Life Tables, Canada population, 2015/2017</t>
-  </si>
-  <si>
-    <t>Life Tables, Ontario population, 2017/2019</t>
-  </si>
-  <si>
-    <t>Life Tables, Ontario population, 2016/2018</t>
-  </si>
-  <si>
-    <t>Life Tables, Ontario population, 2015/2017</t>
-  </si>
-  <si>
-    <t>Life Tables, Québec population, 2017/2019</t>
-  </si>
-  <si>
-    <t>Life Tables, Québec population, 2016/2018</t>
-  </si>
-  <si>
-    <t>Life Tables, Québec population, 2015/2017</t>
   </si>
   <si>
     <t>1971 Group Annuity Mortality (GAM) Table</t>
@@ -926,6 +876,401 @@
       <t>yellow cells</t>
     </r>
   </si>
+  <si>
+    <t>Select a set of mortality tables and projection scales</t>
+  </si>
+  <si>
+    <t>In the 'Annuitants' worksheet, enter the information of the annuitants.  Enter either the age(s) or date(s) of birth.  If you enter the date(s) of birth, enter also the date of calculation.</t>
+  </si>
+  <si>
+    <t>a)</t>
+  </si>
+  <si>
+    <t>b)</t>
+  </si>
+  <si>
+    <t>c)</t>
+  </si>
+  <si>
+    <t>The resulting annuity factor will appear on cell B27.</t>
+  </si>
+  <si>
+    <t>In the 'Annuity factor' worksheet, complete the information for:</t>
+  </si>
+  <si>
+    <t>In the 'Settings' worksheet, select the appropriate options for your regional settings and set of mortality tables.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>annuity characteristics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>: guarantee, % of reversion to co-annuitant, …</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>interest rate(s)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>.  Either CIA 3500 or a vector of interest rate(s) (1, 3, 5 terms vector for 1, 2 and 3 interest rates respectively)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>indexation rate(s)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>.  Either CIA 3500 or a vector of indexation rate(s) (1, 3, 5 terms vector for 1, 2 and 3 interest rates respectively)</t>
+    </r>
+  </si>
+  <si>
+    <t>d)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>mortality assumptions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>.  CIA 3500 assumptions will be used if interest rates have been set to CIA 3500.</t>
+    </r>
+  </si>
+  <si>
+    <t>Life Table, Canada population, 2016/2018</t>
+  </si>
+  <si>
+    <t>Life Table, Canada population, 2017/2019</t>
+  </si>
+  <si>
+    <t>Life Table, Canada population, 2015/2017</t>
+  </si>
+  <si>
+    <t>Life Table, Ontario population, 2017/2019</t>
+  </si>
+  <si>
+    <t>Life Table, Ontario population, 2016/2018</t>
+  </si>
+  <si>
+    <t>Life Table, Ontario population, 2015/2017</t>
+  </si>
+  <si>
+    <t>Life Table, Québec population, 2017/2019</t>
+  </si>
+  <si>
+    <t>Life Table, Québec population, 2016/2018</t>
+  </si>
+  <si>
+    <t>Life Table, Québec population, 2015/2017</t>
+  </si>
+  <si>
+    <t>RP-2014 Rates-Healthy annuitant, Blue Collar</t>
+  </si>
+  <si>
+    <t>RP-2014 Rates-Healthy annuitant, White Collar</t>
+  </si>
+  <si>
+    <t>RP-2014 Rates-Healthy annuitant, Top quartile (benefit)</t>
+  </si>
+  <si>
+    <t>RP-2014 Rates-Healthy annuitant, Bottom quartile (benefit)</t>
+  </si>
+  <si>
+    <t>RP-2014 Rates-Employee, Blue Collar</t>
+  </si>
+  <si>
+    <t>RP-2014 Rates-Employee, White Collar</t>
+  </si>
+  <si>
+    <t>RP-2014 Rates-Employee, Top quartile (salary)</t>
+  </si>
+  <si>
+    <t>RP-2014 Rates-Employee, Bottom quartile (salary)</t>
+  </si>
+  <si>
+    <t>RPH2014A</t>
+  </si>
+  <si>
+    <t>RPH-2014 Rates-Healthy annuitant (Headcount weighted)</t>
+  </si>
+  <si>
+    <t>RPH2014A_BLUE</t>
+  </si>
+  <si>
+    <t>RPH-2014 Rates-Healthy annuitant, Blue Collar (Headcount weighted)</t>
+  </si>
+  <si>
+    <t>RPH2014A_WHITE</t>
+  </si>
+  <si>
+    <t>RPH-2014 Rates-Healthy annuitant, White Collar (Headcount weighted)</t>
+  </si>
+  <si>
+    <t>RPH2014D</t>
+  </si>
+  <si>
+    <t>RPH-2014 Rates-Disabled annuitant (Headcount weighted)</t>
+  </si>
+  <si>
+    <t>RPH2014E</t>
+  </si>
+  <si>
+    <t>RPH-2014 Rates-Employee (Headcount weighted)</t>
+  </si>
+  <si>
+    <t>RPH2014E_BLUE</t>
+  </si>
+  <si>
+    <t>RPH-2014 Rates-Employee, Blue Collar (Headcount weighted)</t>
+  </si>
+  <si>
+    <t>RPH2014E_WHITE</t>
+  </si>
+  <si>
+    <t>RPH-2014 Rates-Employee, White Collar (Headcount weighted)</t>
+  </si>
+  <si>
+    <t>IRC417_2022</t>
+  </si>
+  <si>
+    <t>IRC Section 417(e)(3) Unisex rates for distributions, annuity starting in 2022</t>
+  </si>
+  <si>
+    <t>IRC430_2022A</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2022, Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2022NA</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2022, Non Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2022C</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2022, Combined</t>
+  </si>
+  <si>
+    <t>IRC417_2021</t>
+  </si>
+  <si>
+    <t>IRC Section 417(e)(3) Unisex rates for distributions, annuity starting in 2021</t>
+  </si>
+  <si>
+    <t>IRC430_2021A</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2021, Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2021NA</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2021, Non Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2021C</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2021, Combined</t>
+  </si>
+  <si>
+    <t>IRC417_2020</t>
+  </si>
+  <si>
+    <t>IRC Section 417(e)(3) Unisex rates for distributions, annuity starting in 2020</t>
+  </si>
+  <si>
+    <t>IRC430_2020A</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2020, Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2020NA</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2020, Non Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2020C</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2020, Combined</t>
+  </si>
+  <si>
+    <t>IRC417_2019</t>
+  </si>
+  <si>
+    <t>IRC Section 417(e)(3) Unisex rates for distributions, annuity starting in 2019</t>
+  </si>
+  <si>
+    <t>IRC430_2019A</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2019, Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2019NA</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2019, Non Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2019C</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2019, Combined</t>
+  </si>
+  <si>
+    <t>IRC417_2018</t>
+  </si>
+  <si>
+    <t>IRC Section 417(e)(3) Unisex rates for distributions, annuity starting in 2018</t>
+  </si>
+  <si>
+    <t>IRC430_2018A</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2018, Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2018NA</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2018, Non Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2018C</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2018, Combined</t>
+  </si>
+  <si>
+    <t>IRC417_2017</t>
+  </si>
+  <si>
+    <t>IRC Section 417(e)(3) Unisex rates for distributions, annuity starting in 2017</t>
+  </si>
+  <si>
+    <t>IRC430_2017A</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2017, Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2017NA</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2017, Non Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2017C</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2017, Combined</t>
+  </si>
+  <si>
+    <t>IRC417_2016</t>
+  </si>
+  <si>
+    <t>IRC Section 417(e)(3) Unisex rates for distributions, annuity starting in 2016</t>
+  </si>
+  <si>
+    <t>IRC430_2016A</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2016, Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2016NA</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2016, Non Annuitant</t>
+  </si>
+  <si>
+    <t>IRC430_2016C</t>
+  </si>
+  <si>
+    <t>IRC Section 430(h)(3)(A) Rates for valuation dates in 2016, Combined</t>
+  </si>
+  <si>
+    <t>Annuity Factors Calculator - User guide</t>
+  </si>
 </sst>
 </file>
 
@@ -938,7 +1283,7 @@
     <numFmt numFmtId="167" formatCode="0.00000"/>
     <numFmt numFmtId="168" formatCode="yyyy/mmm"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1121,8 +1466,38 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1174,6 +1549,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1334,7 +1715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1346,33 +1727,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
@@ -1386,17 +1741,6 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
@@ -1499,27 +1843,9 @@
     <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
@@ -1531,9 +1857,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
@@ -1695,9 +2018,6 @@
     <xf numFmtId="10" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" shrinkToFit="1"/>
       <protection locked="0"/>
@@ -1708,18 +2028,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1745,24 +2053,84 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
@@ -1781,11 +2149,57 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2213,6 +2627,212 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1569EDE9-2FA2-4CC4-A941-F634377E6E7C}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="117"/>
+    <col min="2" max="2" width="4.54296875" style="113" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="113"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="126" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+    </row>
+    <row r="3" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="112">
+        <v>1</v>
+      </c>
+      <c r="B3" s="125" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="114"/>
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+    </row>
+    <row r="5" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="112">
+        <v>2</v>
+      </c>
+      <c r="B5" s="125" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="125"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="125"/>
+      <c r="I5" s="125"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="125"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="114"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="112">
+        <v>3</v>
+      </c>
+      <c r="B7" s="127" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="127"/>
+      <c r="J7" s="127"/>
+      <c r="K7" s="127"/>
+    </row>
+    <row r="8" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="116" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="128" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="128"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="128"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="128"/>
+    </row>
+    <row r="9" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="116" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="125" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="125"/>
+      <c r="E9" s="125"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="125"/>
+      <c r="I9" s="125"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="125"/>
+    </row>
+    <row r="10" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="116" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="125" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" s="125"/>
+      <c r="E10" s="125"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="125"/>
+      <c r="H10" s="125"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="125"/>
+    </row>
+    <row r="11" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="116" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="125" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" s="125"/>
+      <c r="E11" s="125"/>
+      <c r="F11" s="125"/>
+      <c r="G11" s="125"/>
+      <c r="H11" s="125"/>
+      <c r="I11" s="125"/>
+      <c r="J11" s="125"/>
+      <c r="K11" s="125"/>
+    </row>
+    <row r="13" spans="1:11" ht="26" x14ac:dyDescent="0.35">
+      <c r="A13" s="129" t="s">
+        <v>193</v>
+      </c>
+      <c r="B13" s="129"/>
+      <c r="C13" s="129"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="129"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="129"/>
+      <c r="J13" s="129"/>
+      <c r="K13" s="129"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="rZVw+i97bLQFfI9k4nzhLjtL16qKIBcy4IYlFy+Z33aNqsfnUnSXnROmlQ+JGETqr3oVidM6y0NAVZTkKAUCNg==" saltValue="WfIRdKU3nGw4aV9qlpLBmA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="9">
+    <mergeCell ref="C9:K9"/>
+    <mergeCell ref="C10:K10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="C8:K8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D606AFD9-149A-46AF-A4DC-CB5AE176F1CC}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFFF00"/>
@@ -2221,580 +2841,568 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.90625" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="52" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="4.7265625" style="64" customWidth="1"/>
-    <col min="5" max="5" width="31.453125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.6328125" style="23" customWidth="1"/>
-    <col min="8" max="10" width="15.6328125" style="24" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.90625" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="24"/>
+    <col min="1" max="1" width="23.90625" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="41" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="4.7265625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="31.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.6328125" style="12" customWidth="1"/>
+    <col min="8" max="10" width="15.6328125" style="13" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.90625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="146" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="70" t="s">
+      <c r="A1" s="134" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
-      <c r="J1" s="147"/>
-      <c r="K1" s="147"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="73">
+      <c r="B3" s="55">
         <v>1</v>
       </c>
-      <c r="C3" s="48" t="str" cm="1">
+      <c r="C3" s="37" t="str" cm="1">
         <f t="array" ref="C3">"&lt;-- "&amp;_z_idMin&amp;" ... "&amp;_z_idMax</f>
         <v>&lt;-- 1 ... 4</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="75" t="str">
+      <c r="B4" s="57" t="str">
         <f>LEFT(_d_name,20)</f>
         <v>Doe, John</v>
       </c>
-      <c r="C4" s="76" t="str">
+      <c r="C4" s="58" t="str">
         <f>IF(_t_errorPerson,"Invalid data","")</f>
         <v/>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="E4" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="75">
+      <c r="B5" s="57">
         <f>_d_sex1</f>
         <v>1</v>
       </c>
-      <c r="E5" s="78" t="s">
+      <c r="E5" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="F5" s="79" t="b">
+      <c r="F5" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="80">
+      <c r="G5" s="62">
         <v>0.03</v>
       </c>
-      <c r="H5" s="81"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="84" t="str">
+      <c r="H5" s="63"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="66" t="str">
         <f>IF(_t_cia_interest_conflict,"CIA and interest conflict",IF(AND(_i_cia_interest_asked,_d_dtCalc=0),"Dt Calc missing",IF(AND(NOT(_t_cia_interest_asked),_i_interestRate1=""),"&lt;-- Rate 1 missing",IF(OR(AND(_i_interestPeriod1&gt;0,_i_interestRate2=""),AND(_i_interestPeriod2&gt;0,_i_interestRate3="")),"&lt;-- Invalid vector",""))))</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="85">
+      <c r="B6" s="67">
         <f>_t_age1</f>
         <v>63</v>
       </c>
-      <c r="E6" s="86"/>
-      <c r="F6" s="69" t="str">
+      <c r="E6" s="68"/>
+      <c r="F6" s="51" t="str">
         <f>IF(_t_cia_interest_show,"CIA "&amp;TEXT(_t_dtCIA,_f_dtCiaShort)&amp;"--&gt;","")</f>
         <v/>
       </c>
-      <c r="G6" s="87" t="str" cm="1">
+      <c r="G6" s="69" t="str" cm="1">
         <f t="array" ref="G6">IF(_t_cia_interest_show,_t_cia_interest,"")</f>
         <v/>
       </c>
-      <c r="H6" s="88"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="89"/>
-      <c r="K6" s="90"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="75" cm="1">
+      <c r="B7" s="57" cm="1">
         <f t="array" ref="B7">_t_sex2_temp</f>
         <v>2</v>
       </c>
-      <c r="D7" s="91"/>
+      <c r="D7" s="73"/>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="85">
+      <c r="B8" s="67">
         <f>_t_age2</f>
         <v>60</v>
       </c>
-      <c r="C8" s="92" t="str">
+      <c r="C8" s="74" t="str">
         <f>IF(AND(_t_hasReversion,B8=""),"&lt;-- Missing","")</f>
         <v/>
       </c>
-      <c r="D8" s="91"/>
-      <c r="E8" s="77" t="s">
+      <c r="D8" s="73"/>
+      <c r="E8" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="K8" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="93">
+      <c r="B9" s="75">
         <f>IF(_d_dtCalc=0,"",_d_dtCalc)</f>
         <v>44505</v>
       </c>
-      <c r="E9" s="78" t="s">
+      <c r="E9" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="F9" s="81" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="82"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="66" t="str">
+      <c r="F9" s="63" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="64"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="49" t="str">
         <f>IF(_cia_indexation_warning,"Warning - CIA assumptions not used",IF(_t_cia_indexation_conflict,"CIA and indexation conflict",IF(AND(_i_cia_indexation_asked,_d_dtCalc=0),"Dt Calc missing",IF(OR(AND(_i_indexationPeriod1&gt;0,_i_indexationRate2=""),AND(_i_indexationPeriod2&gt;0,_i_indexationRate3="")),"&lt;-- Invalid vector",""))))</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E10" s="78"/>
-      <c r="F10" s="115" t="str">
-        <f>IF(_t_cia_interest_show,"CIA "&amp;TEXT(_t_dtCIA,_f_dtCiaShort)&amp;"--&gt;","")</f>
+      <c r="E10" s="60"/>
+      <c r="F10" s="97" t="str">
+        <f>IF(AND(_i_cia_indexation_asked,_e_error5=""),"CIA "&amp;TEXT(_t_dtCIA,_f_dtCiaShort)&amp;"--&gt;","")</f>
         <v/>
       </c>
-      <c r="G10" s="94" cm="1">
-        <f t="array" aca="1" ref="G10:I10" ca="1">IF(_t_cia_indexation_show,_t_cia_indexation,"")</f>
-        <v>1.4055899900391022E-2</v>
-      </c>
-      <c r="H10" s="95">
-        <f ca="1"/>
-        <v>10</v>
-      </c>
-      <c r="I10" s="94">
-        <f ca="1"/>
-        <v>2.0534488581689381E-2</v>
-      </c>
-      <c r="J10" s="96"/>
-      <c r="K10" s="97"/>
+      <c r="G10" s="76" t="str" cm="1">
+        <f t="array" ref="G10">IF(_t_cia_indexation_show,_t_cia_indexation,"")</f>
+        <v/>
+      </c>
+      <c r="H10" s="77"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="79"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="75"/>
-      <c r="E11" s="78" t="s">
+      <c r="B11" s="57"/>
+      <c r="E11" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="98"/>
-      <c r="G11" s="48" t="str" cm="1">
+      <c r="F11" s="80"/>
+      <c r="G11" s="37" t="str" cm="1">
         <f t="array" ref="G11">IF(_i_ageIndexation="","&lt;-- "&amp;TEXT(_t_ageFirstIndexMin+1,_f_dec2),"")</f>
         <v>&lt;-- 64.00</v>
       </c>
-      <c r="H11" s="96"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="97"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="79"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="99"/>
-      <c r="C12" s="48" t="str">
+      <c r="B12" s="81"/>
+      <c r="C12" s="37" t="str">
         <f>IF(_i_guarantee="","&lt;-- "&amp;TEXT(_t_guarantee,_f_dec2),"")</f>
         <v>&lt;-- 0.00</v>
       </c>
-      <c r="E12" s="78" t="s">
+      <c r="E12" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="98"/>
-      <c r="G12" s="48" t="str">
+      <c r="F12" s="80"/>
+      <c r="G12" s="37" t="str">
         <f>IF(_i_fracFirstIndexation="","&lt;-- "&amp;TEXT(1,_f_dec2),"")</f>
         <v>&lt;-- 1.00</v>
       </c>
-      <c r="H12" s="96"/>
-      <c r="I12" s="96"/>
-      <c r="J12" s="96"/>
-      <c r="K12" s="97"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="79"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="100">
-        <v>0.6</v>
-      </c>
-      <c r="C13" s="48" t="str">
+      <c r="B13" s="82"/>
+      <c r="C13" s="37" t="str">
         <f>IF(_i_reversion="","&lt;-- "&amp;TEXT(_t_reversion,_f_perc2),"")</f>
-        <v/>
-      </c>
-      <c r="E13" s="101" t="s">
+        <v>&lt;-- 0.00%</v>
+      </c>
+      <c r="E13" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="F13" s="95"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="96"/>
-      <c r="I13" s="96"/>
-      <c r="J13" s="96"/>
-      <c r="K13" s="97"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="79"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="99"/>
-      <c r="C14" s="48" t="str">
+      <c r="B14" s="81"/>
+      <c r="C14" s="37" t="str">
         <f>IF(_i_deferred="","&lt;-- "&amp;TEXT(_t_deferred,_f_dec2),"")</f>
         <v>&lt;-- 0.00</v>
       </c>
-      <c r="E14" s="78" t="s">
+      <c r="E14" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="F14" s="82"/>
-      <c r="G14" s="43" t="str">
+      <c r="F14" s="64"/>
+      <c r="G14" s="32" t="str">
         <f>IF(_i_indexation_offset="","&lt;-- "&amp;TEXT(0,_f_perc2),"")</f>
         <v>&lt;-- 0.00%</v>
       </c>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="96"/>
-      <c r="K14" s="97"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="79"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="99"/>
-      <c r="C15" s="48" t="str">
+      <c r="B15" s="81"/>
+      <c r="C15" s="37" t="str">
         <f>IF(_i_yearsPaid="","&lt;-- n/a","")</f>
         <v>&lt;-- n/a</v>
       </c>
-      <c r="E15" s="78" t="s">
+      <c r="E15" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="F15" s="82"/>
-      <c r="G15" s="43" t="str">
+      <c r="F15" s="64"/>
+      <c r="G15" s="32" t="str">
         <f>IF(_i_indexation_fraction="","&lt;-- "&amp;TEXT(1,_f_perc2),"")</f>
         <v>&lt;-- 100.00%</v>
       </c>
-      <c r="H15" s="96"/>
-      <c r="I15" s="96"/>
-      <c r="J15" s="96"/>
-      <c r="K15" s="97"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="79"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="103"/>
-      <c r="C16" s="48" t="str">
+      <c r="B16" s="85"/>
+      <c r="C16" s="37" t="str">
         <f>IF(_i_frequency="","&lt;-- "&amp;_t_frequency,"")</f>
         <v>&lt;-- 12</v>
       </c>
-      <c r="E16" s="86" t="s">
+      <c r="E16" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="F16" s="104"/>
-      <c r="G16" s="44" t="str">
+      <c r="F16" s="86"/>
+      <c r="G16" s="33" t="str">
         <f>IF(_i_indexation_max="","&lt;-- "&amp;TEXT(1,_f_perc2),"")</f>
         <v>&lt;-- 100.00%</v>
       </c>
-      <c r="H16" s="89"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="89"/>
-      <c r="K16" s="90"/>
-      <c r="L16" s="105"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="72"/>
+      <c r="L16" s="87"/>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="74" t="s">
+      <c r="A17" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="103"/>
-      <c r="C17" s="48" t="str">
+      <c r="B17" s="85"/>
+      <c r="C17" s="37" t="str">
         <f>IF(_i_due="","&lt;-- "&amp;_t_due,"")</f>
         <v>&lt;-- TRUE</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="74" t="s">
+      <c r="A18" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="103"/>
-      <c r="C18" s="48" t="str">
+      <c r="B18" s="85"/>
+      <c r="C18" s="37" t="str">
         <f>IF(_i_qxPre="","&lt;-- "&amp;_t_qxPre,"")</f>
         <v>&lt;-- TRUE</v>
       </c>
-      <c r="E18" s="77" t="str">
+      <c r="E18" s="59" t="str">
         <f>"Mortality"&amp;IF(_t_cia_interest_show," (CIA 3500)","")</f>
         <v>Mortality</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="106"/>
-      <c r="I18" s="107"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="89"/>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E19" s="78" t="s">
+      <c r="E19" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="136" t="str">
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="131" t="str">
         <f>"&lt;-- "&amp;TEXT(_t_sex1,_f_dec2)&amp;" / "&amp;TEXT(_t_sex2,_f_dec2)</f>
         <v>&lt;-- 1.00 / 2.00</v>
       </c>
-      <c r="I19" s="137"/>
+      <c r="I19" s="132"/>
     </row>
     <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E20" s="78" t="s">
+      <c r="E20" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="108" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" s="108" t="s">
-        <v>89</v>
-      </c>
-      <c r="H20" s="136" t="str">
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="131" t="str">
         <f>"&lt;-- "&amp;_t_qxTable1&amp;" / "&amp;IF(_i_reversion=0,"none",_t_qxTable2)</f>
-        <v>&lt;-- RP2014A / RP2014D</v>
-      </c>
-      <c r="I20" s="136"/>
-      <c r="J20" s="134" t="str">
+        <v>&lt;-- CPM2014 / none</v>
+      </c>
+      <c r="I20" s="131"/>
+      <c r="J20" s="135" t="str">
         <f>IF(_cia_qx_all_valid,"","Invalid under CIA 3500")</f>
         <v/>
       </c>
-      <c r="K20" s="135"/>
+      <c r="K20" s="136"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E21" s="78" t="s">
+      <c r="E21" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="136" t="str">
+      <c r="F21" s="90"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="131" t="str">
         <f>"&lt;-- "&amp;TEXT(_i_qxShitAge1,"0")&amp;" / "&amp;IF(_i_reversion=0,"none",TEXT(_i_qxShitAge2,"0"))</f>
-        <v>&lt;-- 0 / 0</v>
-      </c>
-      <c r="I21" s="137"/>
+        <v>&lt;-- 0 / none</v>
+      </c>
+      <c r="I21" s="132"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D22" s="109"/>
-      <c r="E22" s="78" t="s">
+      <c r="D22" s="91"/>
+      <c r="E22" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="136" t="str">
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="131" t="str">
         <f>"&lt;-- "&amp;TEXT(_i_qxLoading1,_f_perc2)&amp;" / "&amp;IF(_i_reversion=0,"none",TEXT(_i_qxLoading2,_f_perc2))</f>
-        <v>&lt;-- 0.00% / 0.00%</v>
-      </c>
-      <c r="I22" s="137"/>
+        <v>&lt;-- 0.00% / none</v>
+      </c>
+      <c r="I22" s="132"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E23" s="78" t="s">
+      <c r="E23" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="108"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="136" t="str">
+      <c r="F23" s="90"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="131" t="str">
         <f>"&lt;-- "&amp;IF(_t_qxScale1="","none",_t_qxScale1)&amp;" / "&amp;IF(_i_reversion=0,"none",_t_qxScale2)</f>
-        <v xml:space="preserve">&lt;-- none / </v>
-      </c>
-      <c r="I23" s="137"/>
+        <v>&lt;-- none / none</v>
+      </c>
+      <c r="I23" s="132"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E24" s="78" t="s">
+      <c r="E24" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="95" t="str">
+      <c r="F24" s="77" t="str">
         <f>IF(_t_qxProjection1,VLOOKUP(_t_qxTable1,_z_tabQxTable,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="G24" s="95" t="str">
+      <c r="G24" s="77" t="str">
         <f>IF(AND(_t_hasReversion,_t_qxProjection2),VLOOKUP(_t_qxTable2,_z_tabQxTable,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H24" s="96"/>
-      <c r="I24" s="97"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="79"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E25" s="78" t="s">
+      <c r="E25" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="108"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="136" t="str">
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="131" t="str">
         <f>IF(OR(_t_qxProjection1,_t_qxProjection2),"&lt;-- "&amp;_t_qxValuationYear1&amp;" / "&amp;_t_qxValuationYear2,"")</f>
         <v/>
       </c>
-      <c r="I25" s="137"/>
+      <c r="I25" s="132"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E26" s="86" t="s">
+      <c r="E26" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="113" t="str">
+      <c r="F26" s="95" t="str">
         <f>IF(_t_qxProjection1,_t_age1,"")</f>
         <v/>
       </c>
-      <c r="G26" s="113" t="str">
+      <c r="G26" s="95" t="str">
         <f>IF(AND(_t_hasReversion,_t_qxProjection2),_t_age2,"")</f>
         <v/>
       </c>
-      <c r="H26" s="89"/>
-      <c r="I26" s="90"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="72"/>
     </row>
     <row r="27" spans="1:11" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="111" t="s">
+      <c r="A27" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="65" cm="1">
-        <f t="array" aca="1" ref="B27" ca="1">IF(_show_results,IF(_t_hasReversion,_xll.JS(_t_age1,_xll.LX(_t_sex1,_t_qxTable1,_i_qxShitAge1,_i_qxLoading1,_t_qxProjection1,_t_qxScale1,_ic_qxTableBaseYear1,_t_qxValuationYear1,_t_qxAgeValuation1),_t_interestVector,_t_age2,_xll.LX(_t_sex2,_t_qxTable2,_i_qxShitAge2,_i_qxLoading2,_t_qxProjection2,_t_qxScale2,_ic_qxTableBaseYear2,_t_qxValuationYear2,_t_qxAgeValuation2),_t_reversion,_t_guarantee,_t_deferred,_i_yearsPaid,_t_indexationVector,_i_ageIndexation,_t_frequency,_t_due,_t_qxPre,,,_t_fracFirstIndexation),_xll.JS(_t_age1,_xll.LX(_t_sex1,_t_qxTable1,_i_qxShitAge1,_i_qxLoading1,_t_qxProjection1,_t_qxScale1,_ic_qxTableBaseYear1,_t_qxValuationYear1,_t_qxAgeValuation1),_t_interestVector,,,,_t_guarantee,_t_deferred,_i_yearsPaid,_t_indexationVector,_i_ageIndexation,_t_frequency,_t_due,_t_qxPre,,,_t_fracFirstIndexation)),"")</f>
-        <v>20.651311549998891</v>
-      </c>
-      <c r="C27" s="112" t="str">
+      <c r="B27" s="48" cm="1">
+        <f t="array" ref="B27">IF(_show_results,IF(_t_hasReversion,_xll.JS(_t_age1,_xll.LX_aea(_t_sex1,_t_qxTable1,_i_qxShitAge1,_i_qxLoading1,_t_qxProjection1,_t_qxScale1,_ic_qxTableBaseYear1,_t_qxValuationYear1,_t_qxAgeValuation1),_t_interestVector,_t_age2,_xll.LX_aea(_t_sex2,_t_qxTable2,_i_qxShitAge2,_i_qxLoading2,_t_qxProjection2,_t_qxScale2,_ic_qxTableBaseYear2,_t_qxValuationYear2,_t_qxAgeValuation2),_t_reversion,_t_guarantee,_t_deferred,_i_yearsPaid,_t_indexationVector,_i_ageIndexation,_t_frequency,_t_due,_t_qxPre,,,_t_fracFirstIndexation),_xll.JS(_t_age1,_xll.LX_aea(_t_sex1,_t_qxTable1,_i_qxShitAge1,_i_qxLoading1,_t_qxProjection1,_t_qxScale1,_ic_qxTableBaseYear1,_t_qxValuationYear1,_t_qxAgeValuation1),_t_interestVector,,,,_t_guarantee,_t_deferred,_i_yearsPaid,_t_indexationVector,_i_ageIndexation,_t_frequency,_t_due,_t_qxPre,,,_t_fracFirstIndexation)),"")</f>
+        <v>15.869607257140894</v>
+      </c>
+      <c r="C27" s="94" t="str">
         <f>IF(_settings_invalid,"Invalid settings",IF(_cia_warning,"Warning - CIA",IF(_t_errorSomewhere,"Invalid input","")))</f>
         <v/>
       </c>
-      <c r="E27" s="114"/>
+      <c r="E27" s="96"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E28" s="131" t="s">
+      <c r="E28" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="133" t="s">
+      <c r="F28" s="110" t="s">
         <v>157</v>
       </c>
-      <c r="G28" s="74"/>
-      <c r="H28" s="132"/>
-      <c r="I28" s="132"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="109"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="72" t="s">
+      <c r="A29" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="B29" s="139" t="s">
+      <c r="B29" s="133" t="s">
         <v>151</v>
       </c>
-      <c r="C29" s="139"/>
-      <c r="E29" s="72" t="str">
+      <c r="C29" s="133"/>
+      <c r="E29" s="54" t="str">
         <f>_t_qxTable1</f>
-        <v>RP2014A</v>
-      </c>
-      <c r="F29" s="138" t="str">
+        <v>CPM2014</v>
+      </c>
+      <c r="F29" s="130" t="str">
         <f>_t_qxTable1Descr</f>
-        <v>RP-2014 Rates-Healthy annuitant</v>
-      </c>
-      <c r="G29" s="138"/>
-      <c r="H29" s="138"/>
-      <c r="I29" s="138"/>
+        <v>Canadian Pensioners’ Mortality (CPM) 2014, composite of Public and Private Sector</v>
+      </c>
+      <c r="G29" s="130"/>
+      <c r="H29" s="130"/>
+      <c r="I29" s="130"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="72" t="s">
+      <c r="A30" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="139" t="str" cm="1">
+      <c r="B30" s="133" t="str" cm="1">
         <f t="array" ref="B30">"version "&amp;_xll.version_aea()</f>
         <v>version 4.5.3</v>
       </c>
-      <c r="C30" s="139"/>
-      <c r="E30" s="72" t="str">
+      <c r="C30" s="133"/>
+      <c r="E30" s="54" t="str">
         <f>IF(OR(_t_qxTable2="",_t_qxTable2=_t_qxTable1),"",_t_qxTable2)</f>
-        <v>RP2014D</v>
-      </c>
-      <c r="F30" s="138" t="str">
+        <v/>
+      </c>
+      <c r="F30" s="130" t="str">
         <f>IF(OR(_t_qxTable2="",_t_qxTable2=_t_qxTable1),"",_t_qxTable2Descr)</f>
-        <v>RP-2014 Rates-Disabled annuitant</v>
-      </c>
-      <c r="G30" s="138"/>
-      <c r="H30" s="138"/>
-      <c r="I30" s="138"/>
+        <v/>
+      </c>
+      <c r="G30" s="130"/>
+      <c r="H30" s="130"/>
+      <c r="I30" s="130"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Acmy2aElRFFWrtZgw7Kk/W2jM3HL1tMIG9uNHz/stjq4wHuf3mkn7Q8xmFVGlxYzbvi/F8jWorQWt3t6oiCUZQ==" saltValue="UMGoZbTvkKzGhZrYKzQBXw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="12">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="F29:I29"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="F6">
@@ -2920,7 +3528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A5EC3D-B72E-47B1-B0A7-90F271932891}">
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FFFFFF00"/>
@@ -2930,213 +3538,213 @@
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B29" sqref="B29"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="6"/>
-    <col min="2" max="2" width="14.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="7"/>
-    <col min="4" max="4" width="8.7265625" style="6"/>
-    <col min="5" max="5" width="8.7265625" style="7"/>
-    <col min="6" max="6" width="8.7265625" style="6"/>
-    <col min="7" max="9" width="11.6328125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="146"/>
+    <col min="2" max="2" width="14.7265625" style="146" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="147"/>
+    <col min="4" max="4" width="8.7265625" style="146"/>
+    <col min="5" max="5" width="8.7265625" style="147"/>
+    <col min="6" max="6" width="8.7265625" style="146"/>
+    <col min="7" max="9" width="11.6328125" style="148" customWidth="1"/>
     <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="151" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-    </row>
-    <row r="2" spans="1:9" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A2" s="60" t="s">
+      <c r="B1" s="152"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+    </row>
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A2" s="155" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-    </row>
-    <row r="3" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" s="11">
+      <c r="B2" s="152"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="156"/>
+      <c r="B3" s="156"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="156"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="143"/>
+      <c r="B4" s="144">
         <f>COLUMN()</f>
         <v>2</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="144">
         <f>COLUMN()</f>
         <v>3</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="144">
         <f>COLUMN()</f>
         <v>4</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="144">
         <f>COLUMN()</f>
         <v>5</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="144">
         <f>COLUMN()</f>
         <v>6</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="144">
         <f>COLUMN()</f>
         <v>7</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="144">
         <f>COLUMN()</f>
         <v>8</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="144">
         <f>COLUMN()</f>
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="149" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="150" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="150" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="149" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="20">
+      <c r="A6" s="145">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="146" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="145">
         <v>63</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="146">
         <v>1</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="147">
         <v>60</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="146">
         <v>2</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="148">
         <v>44505</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="146">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="146" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="147">
         <v>60</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="146">
         <v>2</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="147">
         <v>63</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="146">
         <v>1</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="148">
         <f ca="1">_t_today</f>
-        <v>44511</v>
+        <v>44512</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="146">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="146" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="146">
         <v>1</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="146">
         <v>2</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="148">
         <v>23598</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="148">
         <v>21655</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="148">
         <f ca="1">_t_today</f>
-        <v>44511</v>
+        <v>44512</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="146">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="146" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="146">
         <v>2</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="148">
         <v>22743</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="148">
         <f ca="1">_t_today</f>
-        <v>44511</v>
+        <v>44512</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="REqwDFAZyH9ICo8Fo0OJNLQehELefswmWTJgmUf6fi8v05EbxX2Yt3CYdcyY3afyuSwwwYUfE6Gp6rmHIh3XSA==" saltValue="vKIiLiD86ucKJGtDy9hQHA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4xvB5eYA1kXWiupO04vwE0ogvBFKzy/CP4POdNmhDX6YJ0dUwOyxQh4DSH4nfsIM6anmY6vFp5UIYa7CnuZTxQ==" saltValue="6W6e/4GGF7g6d1AuOa/4DQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations xWindow="444" yWindow="596" count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be 1 or 2." prompt="1 for male, 2 for female." sqref="F1:F1048576 D1:D1048576" xr:uid="{E25F2585-A7E1-4EC5-BB92-EB43A57F46D4}">
       <formula1>1</formula1>
@@ -3152,203 +3760,217 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5A63EB-A2E7-4F8F-BAE1-69D01836B4E9}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="11.26953125" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.6328125" style="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.6328125" style="52" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="24"/>
+    <col min="1" max="1" width="16.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.6328125" style="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.6328125" style="41" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="142" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
+      <c r="A1" s="139" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
     </row>
     <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="137" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="140"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="141" t="s">
+      <c r="A4" s="138" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="141"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
-    </row>
-    <row r="5" spans="1:9" s="64" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="119"/>
-      <c r="B5" s="120" t="str">
+      <c r="B4" s="138"/>
+      <c r="C4" s="138"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+    </row>
+    <row r="5" spans="1:9" s="47" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="100"/>
+      <c r="B5" s="101" t="str">
         <f>IF(_f_language="","error","")</f>
         <v/>
       </c>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-    </row>
-    <row r="6" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+    </row>
+    <row r="6" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="B6" s="118" t="s">
+      <c r="B6" s="99" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="40">
         <f>ROW()-1</f>
         <v>5</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="43" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="52" t="str">
+      <c r="B7" s="41" t="str">
         <f>HLOOKUP(_f_language,_tabFormat,ROW()-_tabFormatOffset,FALSE)</f>
         <v>0.00</v>
       </c>
-      <c r="D7" s="52" t="str">
+      <c r="D7" s="41" t="str">
         <f>"0.00"</f>
         <v>0.00</v>
       </c>
-      <c r="E7" s="52" t="str">
+      <c r="E7" s="41" t="str">
         <f>"0,00"</f>
         <v>0,00</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B8" s="52" t="str">
+      <c r="B8" s="41" t="str">
         <f>HLOOKUP(_f_language,_tabFormat,ROW()-_tabFormatOffset,FALSE)</f>
         <v>0.00%</v>
       </c>
-      <c r="D8" s="52" t="str">
+      <c r="D8" s="41" t="str">
         <f>"0.00%"</f>
         <v>0.00%</v>
       </c>
-      <c r="E8" s="52" t="str">
+      <c r="E8" s="41" t="str">
         <f>"0,00%"</f>
         <v>0,00%</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="52" t="str">
+      <c r="B9" s="41" t="str">
         <f>HLOOKUP(_f_language,_tabFormat,ROW()-_tabFormatOffset,FALSE)</f>
         <v>yyyy-mmmm</v>
       </c>
-      <c r="D9" s="52" t="str">
+      <c r="D9" s="41" t="str">
         <f>"yyyy-mmmm"</f>
         <v>yyyy-mmmm</v>
       </c>
-      <c r="E9" s="52" t="str">
+      <c r="E9" s="41" t="str">
         <f>"aaaa-mmmm"</f>
         <v>aaaa-mmmm</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B10" s="52" t="str">
+      <c r="B10" s="41" t="str">
         <f>HLOOKUP(_f_language,_tabFormat,ROW()-_tabFormatOffset,FALSE)</f>
         <v>yyyy-mm</v>
       </c>
-      <c r="D10" s="52" t="str">
+      <c r="D10" s="41" t="str">
         <f>"yyyy-mm"</f>
         <v>yyyy-mm</v>
       </c>
-      <c r="E10" s="52" t="str">
+      <c r="E10" s="41" t="str">
         <f>"aaaa-mm"</f>
         <v>aaaa-mm</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="112" t="str">
+    <row r="13" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="137" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" s="137"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="137"/>
+      <c r="E13" s="137"/>
+      <c r="F13" s="137"/>
+      <c r="G13" s="137"/>
+      <c r="H13" s="137"/>
+      <c r="I13" s="137"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="11"/>
+      <c r="B14" s="94" t="str">
         <f>IF(_s_country="","error","")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="22" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="117" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="22" t="s">
+      <c r="B15" s="99" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B16" s="52" t="b">
+      <c r="B18" s="41" t="b">
         <f>OR(_s_error1&lt;&gt;"",_s_error2&lt;&gt;"")</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="3">
+  <sheetProtection algorithmName="SHA-512" hashValue="C2WYvnIlJyo7a2k6zljejXA5r6p8zvGohkfYVswe5uq4DJuwV4ES8syt70N5LOoN87Y2trBmYmS14h2SyxrHnA==" saltValue="+mPRdlyjYsaAVZa9FggAIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <mergeCells count="4">
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A13:I13"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" showErrorMessage="1" error="English or Français" prompt="Language is E or F" sqref="B6" xr:uid="{B2CF9995-1F71-4671-AC15-78E069A549C7}">
       <formula1>_listLanguages</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" error="Invalid country" sqref="B13" xr:uid="{BA89C1AC-526E-4A6B-8466-A80EA131379D}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" error="Invalid country" sqref="B15" xr:uid="{BA89C1AC-526E-4A6B-8466-A80EA131379D}">
       <formula1>_listCountry</formula1>
     </dataValidation>
   </dataValidations>
@@ -3357,17 +3979,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9677B0E8-189A-4E7A-B411-01EEFB116BEC}">
   <sheetPr codeName="Sheet6">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G24" sqref="G24"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3376,85 +3998,85 @@
     <col min="2" max="2" width="11.54296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" style="1"/>
     <col min="4" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7265625" style="2"/>
-    <col min="8" max="8" width="14.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="2" customWidth="1"/>
-    <col min="10" max="10" width="68.453125" style="128" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" style="2" customWidth="1"/>
-    <col min="14" max="14" width="48.7265625" style="128" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" style="105" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="120" customWidth="1"/>
+    <col min="10" max="10" width="68.453125" style="105" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.36328125" style="105" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" style="105" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" style="120" customWidth="1"/>
+    <col min="14" max="14" width="62.26953125" style="105" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.36328125" style="105" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H1" s="143" t="s">
+      <c r="H1" s="140" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="143"/>
-      <c r="J1" s="143"/>
-      <c r="K1" s="143"/>
-      <c r="L1" s="144" t="s">
+      <c r="I1" s="140"/>
+      <c r="J1" s="140"/>
+      <c r="K1" s="140"/>
+      <c r="L1" s="141" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
-      <c r="O1" s="144"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
+      <c r="O1" s="141"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="124" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="62" t="s">
+      <c r="I2" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="129" t="s">
+      <c r="J2" s="106" t="s">
         <v>157</v>
       </c>
-      <c r="K2" s="47" t="s">
+      <c r="K2" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="123" t="s">
+      <c r="L2" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="124" t="s">
+      <c r="M2" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="125" t="s">
+      <c r="N2" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="O2" s="123" t="s">
+      <c r="O2" s="122" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="107" t="s">
         <v>154</v>
       </c>
-      <c r="B3" s="130" t="s">
-        <v>180</v>
+      <c r="B3" s="107" t="s">
+        <v>172</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>135</v>
@@ -3471,19 +4093,19 @@
       <c r="G3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="126"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="126"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="119"/>
+      <c r="J3" s="103"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="103"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="130" t="s">
+      <c r="A4" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="130" t="s">
-        <v>181</v>
+      <c r="B4" s="107" t="s">
+        <v>173</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>136</v>
@@ -3500,28 +4122,28 @@
       <c r="G4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="67">
+      <c r="I4" s="119">
         <v>2014</v>
       </c>
-      <c r="J4" s="126" t="s">
-        <v>195</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="J4" s="103" t="s">
+        <v>178</v>
+      </c>
+      <c r="K4" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="123" t="s">
         <v>86</v>
       </c>
-      <c r="M4" s="67">
+      <c r="M4" s="119">
         <v>2014</v>
       </c>
-      <c r="N4" s="126" t="s">
-        <v>164</v>
-      </c>
-      <c r="O4" s="2" t="s">
+      <c r="N4" s="103" t="s">
+        <v>162</v>
+      </c>
+      <c r="O4" s="105" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3532,28 +4154,28 @@
       <c r="F5" s="2">
         <v>24</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="I5" s="67">
+      <c r="H5" s="123" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" s="119">
         <v>2014</v>
       </c>
-      <c r="J5" s="126" t="s">
-        <v>198</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="J5" s="103" t="s">
+        <v>181</v>
+      </c>
+      <c r="K5" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="123" t="s">
         <v>87</v>
       </c>
-      <c r="M5" s="67">
+      <c r="M5" s="119">
         <v>2014</v>
       </c>
-      <c r="N5" s="126" t="s">
-        <v>165</v>
-      </c>
-      <c r="O5" s="2" t="s">
+      <c r="N5" s="103" t="s">
+        <v>210</v>
+      </c>
+      <c r="O5" s="105" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3565,60 +4187,60 @@
       <c r="F6" s="2">
         <v>26</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="I6" s="67">
+      <c r="H6" s="123" t="s">
+        <v>180</v>
+      </c>
+      <c r="I6" s="119">
         <v>2014</v>
       </c>
-      <c r="J6" s="126" t="s">
-        <v>199</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="J6" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="K6" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="123" t="s">
         <v>88</v>
       </c>
-      <c r="M6" s="67">
+      <c r="M6" s="119">
         <v>2014</v>
       </c>
-      <c r="N6" s="126" t="s">
-        <v>166</v>
-      </c>
-      <c r="O6" s="2" t="s">
+      <c r="N6" s="103" t="s">
+        <v>211</v>
+      </c>
+      <c r="O6" s="105" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="E7" s="17">
+      <c r="E7" s="9">
         <v>0.75</v>
       </c>
       <c r="F7" s="2">
         <v>52</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="67">
+      <c r="I7" s="119">
         <v>1994</v>
       </c>
-      <c r="J7" s="126" t="s">
-        <v>194</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="J7" s="103" t="s">
+        <v>177</v>
+      </c>
+      <c r="K7" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M7" s="67">
+      <c r="L7" s="123" t="s">
+        <v>164</v>
+      </c>
+      <c r="M7" s="119">
         <v>2014</v>
       </c>
-      <c r="N7" s="126" t="s">
-        <v>174</v>
-      </c>
-      <c r="O7" s="2" t="s">
+      <c r="N7" s="103" t="s">
+        <v>212</v>
+      </c>
+      <c r="O7" s="105" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3626,322 +4248,644 @@
       <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="67">
+      <c r="I8" s="119">
         <v>2015</v>
       </c>
-      <c r="J8" s="126" t="s">
-        <v>200</v>
-      </c>
-      <c r="K8" s="2" t="s">
+      <c r="J8" s="103" t="s">
+        <v>183</v>
+      </c>
+      <c r="K8" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="123" t="s">
+        <v>165</v>
+      </c>
+      <c r="M8" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N8" s="103" t="s">
+        <v>213</v>
+      </c>
+      <c r="O8" s="105" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H9" s="123" t="s">
+        <v>185</v>
+      </c>
+      <c r="I9" s="119">
+        <v>2020</v>
+      </c>
+      <c r="J9" s="103" t="s">
+        <v>184</v>
+      </c>
+      <c r="K9" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="123" t="s">
+        <v>89</v>
+      </c>
+      <c r="M9" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N9" s="103" t="s">
+        <v>163</v>
+      </c>
+      <c r="O9" s="105" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H10" s="123" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="119">
+        <v>1983</v>
+      </c>
+      <c r="J10" s="103" t="s">
+        <v>175</v>
+      </c>
+      <c r="K10" s="105" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="123" t="s">
+        <v>83</v>
+      </c>
+      <c r="M10" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N10" s="103" t="s">
+        <v>161</v>
+      </c>
+      <c r="O10" s="105" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H11" s="123" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="119">
+        <v>1983</v>
+      </c>
+      <c r="J11" s="103" t="s">
+        <v>176</v>
+      </c>
+      <c r="K11" s="105" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="123" t="s">
+        <v>85</v>
+      </c>
+      <c r="M11" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N11" s="103" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H12" s="123" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="119">
+        <v>1971</v>
+      </c>
+      <c r="J12" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="L12" s="123" t="s">
+        <v>84</v>
+      </c>
+      <c r="M12" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N12" s="103" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H13" s="123" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="119">
+        <v>2019</v>
+      </c>
+      <c r="J13" s="103" t="s">
+        <v>202</v>
+      </c>
+      <c r="L13" s="123" t="s">
+        <v>166</v>
+      </c>
+      <c r="M13" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N13" s="103" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H14" s="123" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="119">
+        <v>2018</v>
+      </c>
+      <c r="J14" s="103" t="s">
+        <v>201</v>
+      </c>
+      <c r="L14" s="123" t="s">
+        <v>167</v>
+      </c>
+      <c r="M14" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N14" s="103" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H15" s="123" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="119">
+        <v>2017</v>
+      </c>
+      <c r="J15" s="103" t="s">
+        <v>203</v>
+      </c>
+      <c r="L15" s="123" t="s">
+        <v>218</v>
+      </c>
+      <c r="M15" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N15" s="103" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H16" s="123" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="119">
+        <v>2019</v>
+      </c>
+      <c r="J16" s="103" t="s">
+        <v>204</v>
+      </c>
+      <c r="L16" s="123" t="s">
+        <v>220</v>
+      </c>
+      <c r="M16" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N16" s="103" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H17" s="123" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="119">
+        <v>2018</v>
+      </c>
+      <c r="J17" s="103" t="s">
+        <v>205</v>
+      </c>
+      <c r="L17" s="123" t="s">
+        <v>222</v>
+      </c>
+      <c r="M17" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N17" s="103" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H18" s="123" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="119">
+        <v>2017</v>
+      </c>
+      <c r="J18" s="103" t="s">
+        <v>206</v>
+      </c>
+      <c r="L18" s="123" t="s">
+        <v>224</v>
+      </c>
+      <c r="M18" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N18" s="103" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H19" s="123" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="119">
+        <v>2019</v>
+      </c>
+      <c r="J19" s="103" t="s">
+        <v>207</v>
+      </c>
+      <c r="L19" s="123" t="s">
+        <v>226</v>
+      </c>
+      <c r="M19" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N19" s="103" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H20" s="123" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" s="119">
+        <v>2018</v>
+      </c>
+      <c r="J20" s="103" t="s">
+        <v>208</v>
+      </c>
+      <c r="L20" s="123" t="s">
+        <v>228</v>
+      </c>
+      <c r="M20" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N20" s="103" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H21" s="123" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="119">
+        <v>2017</v>
+      </c>
+      <c r="J21" s="103" t="s">
+        <v>209</v>
+      </c>
+      <c r="L21" s="123" t="s">
+        <v>230</v>
+      </c>
+      <c r="M21" s="119">
+        <v>2014</v>
+      </c>
+      <c r="N21" s="103" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="J22" s="104"/>
+      <c r="L22" s="123" t="s">
+        <v>232</v>
+      </c>
+      <c r="M22" s="119">
+        <v>2022</v>
+      </c>
+      <c r="N22" s="103" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="J23" s="104"/>
+      <c r="L23" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="M23" s="119">
+        <v>2022</v>
+      </c>
+      <c r="N23" s="103" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="J24" s="104"/>
+      <c r="L24" s="123" t="s">
+        <v>236</v>
+      </c>
+      <c r="M24" s="119">
+        <v>2022</v>
+      </c>
+      <c r="N24" s="103" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="J25" s="104"/>
+      <c r="L25" s="123" t="s">
+        <v>238</v>
+      </c>
+      <c r="M25" s="119">
+        <v>2022</v>
+      </c>
+      <c r="N25" s="103" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="J26" s="104"/>
+      <c r="L26" s="123" t="s">
+        <v>240</v>
+      </c>
+      <c r="M26" s="119">
+        <v>2021</v>
+      </c>
+      <c r="N26" s="103" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="J27" s="104"/>
+      <c r="L27" s="123" t="s">
+        <v>242</v>
+      </c>
+      <c r="M27" s="119">
+        <v>2021</v>
+      </c>
+      <c r="N27" s="103" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="L28" s="123" t="s">
+        <v>244</v>
+      </c>
+      <c r="M28" s="119">
+        <v>2021</v>
+      </c>
+      <c r="N28" s="103" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="L29" s="123" t="s">
+        <v>246</v>
+      </c>
+      <c r="M29" s="119">
+        <v>2021</v>
+      </c>
+      <c r="N29" s="103" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="L30" s="123" t="s">
+        <v>248</v>
+      </c>
+      <c r="M30" s="119">
+        <v>2020</v>
+      </c>
+      <c r="N30" s="103" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="L31" s="123" t="s">
+        <v>250</v>
+      </c>
+      <c r="M31" s="119">
+        <v>2020</v>
+      </c>
+      <c r="N31" s="103" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="32" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="L32" s="123" t="s">
+        <v>252</v>
+      </c>
+      <c r="M32" s="119">
+        <v>2020</v>
+      </c>
+      <c r="N32" s="103" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="33" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L33" s="123" t="s">
+        <v>254</v>
+      </c>
+      <c r="M33" s="119">
+        <v>2020</v>
+      </c>
+      <c r="N33" s="103" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L34" s="123" t="s">
+        <v>256</v>
+      </c>
+      <c r="M34" s="119">
+        <v>2019</v>
+      </c>
+      <c r="N34" s="103" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L35" s="123" t="s">
+        <v>258</v>
+      </c>
+      <c r="M35" s="119">
+        <v>2019</v>
+      </c>
+      <c r="N35" s="103" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L36" s="123" t="s">
+        <v>260</v>
+      </c>
+      <c r="M36" s="119">
+        <v>2019</v>
+      </c>
+      <c r="N36" s="103" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L37" s="123" t="s">
+        <v>262</v>
+      </c>
+      <c r="M37" s="119">
+        <v>2019</v>
+      </c>
+      <c r="N37" s="103" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L38" s="123" t="s">
+        <v>264</v>
+      </c>
+      <c r="M38" s="119">
+        <v>2018</v>
+      </c>
+      <c r="N38" s="103" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="39" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L39" s="123" t="s">
+        <v>266</v>
+      </c>
+      <c r="M39" s="119">
+        <v>2018</v>
+      </c>
+      <c r="N39" s="103" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="40" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L40" s="123" t="s">
+        <v>268</v>
+      </c>
+      <c r="M40" s="119">
+        <v>2018</v>
+      </c>
+      <c r="N40" s="103" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L41" s="123" t="s">
+        <v>270</v>
+      </c>
+      <c r="M41" s="119">
+        <v>2018</v>
+      </c>
+      <c r="N41" s="103" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="42" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L42" s="123" t="s">
+        <v>272</v>
+      </c>
+      <c r="M42" s="119">
+        <v>2017</v>
+      </c>
+      <c r="N42" s="103" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L43" s="123" t="s">
+        <v>274</v>
+      </c>
+      <c r="M43" s="119">
+        <v>2017</v>
+      </c>
+      <c r="N43" s="103" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L44" s="123" t="s">
+        <v>276</v>
+      </c>
+      <c r="M44" s="119">
+        <v>2017</v>
+      </c>
+      <c r="N44" s="103" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L45" s="123" t="s">
+        <v>278</v>
+      </c>
+      <c r="M45" s="119">
+        <v>2017</v>
+      </c>
+      <c r="N45" s="103" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="46" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L46" s="123" t="s">
+        <v>280</v>
+      </c>
+      <c r="M46" s="119">
+        <v>2016</v>
+      </c>
+      <c r="N46" s="103" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="47" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L47" s="123" t="s">
+        <v>282</v>
+      </c>
+      <c r="M47" s="119">
+        <v>2016</v>
+      </c>
+      <c r="N47" s="103" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L48" s="123" t="s">
+        <v>284</v>
+      </c>
+      <c r="M48" s="119">
+        <v>2016</v>
+      </c>
+      <c r="N48" s="103" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="49" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L49" s="123" t="s">
+        <v>286</v>
+      </c>
+      <c r="M49" s="119">
+        <v>2016</v>
+      </c>
+      <c r="N49" s="103" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="50" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L50" s="123" t="s">
+        <v>73</v>
+      </c>
+      <c r="M50" s="119">
+        <v>2019</v>
+      </c>
+      <c r="N50" s="103" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L51" s="123" t="s">
+        <v>72</v>
+      </c>
+      <c r="M51" s="119">
+        <v>2017</v>
+      </c>
+      <c r="N51" s="103" t="s">
         <v>169</v>
       </c>
-      <c r="M8" s="67">
-        <v>2014</v>
-      </c>
-      <c r="N8" s="126" t="s">
-        <v>175</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H9" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="I9" s="67">
-        <v>2020</v>
-      </c>
-      <c r="J9" s="126" t="s">
-        <v>201</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="M9" s="67">
-        <v>2014</v>
-      </c>
-      <c r="N9" s="126" t="s">
-        <v>167</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="67">
-        <v>1983</v>
-      </c>
-      <c r="J10" s="126" t="s">
-        <v>192</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="M10" s="67">
-        <v>2014</v>
-      </c>
-      <c r="N10" s="126" t="s">
-        <v>161</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H11" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I11" s="67">
-        <v>1983</v>
-      </c>
-      <c r="J11" s="126" t="s">
-        <v>193</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="M11" s="67">
-        <v>2014</v>
-      </c>
-      <c r="N11" s="126" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="67">
-        <v>1971</v>
-      </c>
-      <c r="J12" s="126" t="s">
-        <v>191</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M12" s="67">
-        <v>2014</v>
-      </c>
-      <c r="N12" s="126" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="I13" s="67">
-        <v>2019</v>
-      </c>
-      <c r="J13" s="126" t="s">
-        <v>182</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="M13" s="67">
-        <v>2014</v>
-      </c>
-      <c r="N13" s="126" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H14" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="67">
-        <v>2018</v>
-      </c>
-      <c r="J14" s="126" t="s">
-        <v>183</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="M14" s="67">
-        <v>2014</v>
-      </c>
-      <c r="N14" s="126" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H15" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I15" s="67">
-        <v>2017</v>
-      </c>
-      <c r="J15" s="126" t="s">
-        <v>184</v>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="M15" s="67">
-        <v>2019</v>
-      </c>
-      <c r="N15" s="126" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H16" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" s="67">
-        <v>2019</v>
-      </c>
-      <c r="J16" s="126" t="s">
-        <v>185</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="M16" s="67">
-        <v>2017</v>
-      </c>
-      <c r="N16" s="126" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I17" s="67">
-        <v>2018</v>
-      </c>
-      <c r="J17" s="126" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H18" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I18" s="67">
-        <v>2017</v>
-      </c>
-      <c r="J18" s="126" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="19" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" s="67">
-        <v>2019</v>
-      </c>
-      <c r="J19" s="126" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="20" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I20" s="67">
-        <v>2018</v>
-      </c>
-      <c r="J20" s="126" t="s">
-        <v>189</v>
-      </c>
-      <c r="L20" s="122"/>
-      <c r="M20" s="121"/>
-      <c r="N20" s="127"/>
-    </row>
-    <row r="21" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H21" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I21" s="67">
-        <v>2017</v>
-      </c>
-      <c r="J21" s="126" t="s">
-        <v>190</v>
-      </c>
-      <c r="L21" s="122"/>
-      <c r="M21" s="121"/>
-      <c r="N21" s="127"/>
-    </row>
-    <row r="22" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="127"/>
-      <c r="L22" s="122"/>
-      <c r="M22" s="121"/>
-      <c r="N22" s="127"/>
-    </row>
-    <row r="23" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="127"/>
-      <c r="L23" s="122"/>
-      <c r="M23" s="121"/>
-      <c r="N23" s="127"/>
-    </row>
-    <row r="24" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="127"/>
-      <c r="L24" s="122"/>
-      <c r="M24" s="121"/>
-      <c r="N24" s="127"/>
-    </row>
-    <row r="25" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="127"/>
-      <c r="L25" s="122"/>
-      <c r="M25" s="121"/>
-      <c r="N25" s="127"/>
-    </row>
-    <row r="26" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="127"/>
-      <c r="L26" s="122"/>
-      <c r="M26" s="121"/>
-      <c r="N26" s="127"/>
-    </row>
-    <row r="27" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="127"/>
-      <c r="L27" s="122"/>
-      <c r="M27" s="121"/>
-      <c r="N27" s="127"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="vWLH1gEtFJJI3fiq6706U8Ant6iNZtcsgfmcaB24JolFEr2QKOELK3UZCJYgkwwyz/DcJ+eNgxA01FizmxJESg==" saltValue="w6PQz8kTcA34duxMHmDHbw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:O1"/>
@@ -3952,808 +4896,808 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DA9975-C858-45BF-AEA5-59BD3B014198}">
   <sheetPr codeName="Sheet5">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.36328125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="23" customWidth="1"/>
-    <col min="3" max="5" width="15.6328125" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="24"/>
+    <col min="1" max="1" width="49.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="12" customWidth="1"/>
+    <col min="3" max="5" width="15.6328125" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="23">
+      <c r="B1" s="12">
         <f>_id</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="B2" s="23" t="str">
+      <c r="A2" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="12" t="str">
         <f>VLOOKUP(_s_country,_tabCountry,2,FALSE)</f>
-        <v>USA</v>
+        <v>CAN</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="str">
+      <c r="B3" s="12" t="str">
         <f>VLOOKUP(_id,_tabPersons,_colName,FALSE)</f>
         <v>Doe, John</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="12">
         <f>VLOOKUP(_id,_tabPersons,_colSex1,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="14">
         <f>VLOOKUP(_id,_tabPersons,_colAge1,FALSE)</f>
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="12">
         <f>VLOOKUP(_id,_tabPersons,_colSex2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="31">
         <f>IF(_t_age2="","",IF(_d_sex2=0,3-_d_sex1,_d_sex2))</f>
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="14">
         <f>VLOOKUP(_id,_tabPersons,_colAge2,FALSE)</f>
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="15">
         <f>VLOOKUP(_id,_tabPersons,_colDtBirth1,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C8" s="44">
         <f>IF(AND(_d_dtBirth1&gt;0,_d_dtCalc&gt;0),YEARFRAC(_d_dtBirth1,_d_dtCalc),_d_age1)</f>
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="15">
         <f>VLOOKUP(_id,_tabPersons,_colDtBirth2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="C9" s="55">
+      <c r="C9" s="44">
         <f>IF(AND(_d_age2=0,_d_dtBirth2=0),"",IF(AND(_d_dtBirth2&gt;0,_d_dtCalc&gt;0),YEARFRAC(_d_dtBirth2,_d_dtCalc),_d_age2))</f>
         <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="15">
         <f>VLOOKUP(_id,_tabPersons,_colDtCalc,FALSE)</f>
         <v>44505</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29" t="s">
+      <c r="E11" s="18"/>
+      <c r="F11" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="30" t="b">
+      <c r="B12" s="19" t="b">
         <f>NOT(AND(C12:I12))</f>
         <v>0</v>
       </c>
-      <c r="C12" s="29" t="b">
+      <c r="C12" s="18" t="b">
         <f>_d_sex1&lt;&gt;0</f>
         <v>1</v>
       </c>
-      <c r="D12" s="29" t="b">
+      <c r="D12" s="18" t="b">
         <f>OR(_d_age1&lt;&gt;0,_d_dtBirth1&lt;&gt;0)</f>
         <v>1</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29" t="b">
+      <c r="E12" s="18"/>
+      <c r="F12" s="18" t="b">
         <f>OR(_d_age1,AND(_d_dtCalc&lt;&gt;0,_d_dtBirth1&lt;&gt;0))</f>
         <v>1</v>
       </c>
-      <c r="G12" s="29" t="b">
+      <c r="G12" s="18" t="b">
         <f>OR(_d_sex2&lt;&gt;0,AND(_d_age2=0,_d_dtBirth2=0))</f>
         <v>1</v>
       </c>
-      <c r="H12" s="29" t="b">
+      <c r="H12" s="18" t="b">
         <f>OR(AND(_d_sex2=0,_d_age2=0,_d_dtBirth2=0),_d_age2&lt;&gt;0,_d_dtBirth2&lt;&gt;0)</f>
         <v>1</v>
       </c>
-      <c r="I12" s="29" t="b">
+      <c r="I12" s="18" t="b">
         <f>OR(_d_age2&lt;&gt;0,AND(_d_dtCalc&lt;&gt;0,_d_dtBirth2&lt;&gt;0),AND(_d_sex2=0,_d_age2=0,_d_dtBirth2=0))</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="23" t="b">
+      <c r="B14" s="12" t="b">
         <f>_i_reversion&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="23" t="b">
+      <c r="B15" s="12" t="b">
         <f>OR(_i_indexationRate1&gt;0,_i_indexationRate2&gt;0,_i_indexationRate3&gt;0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="23" t="b">
+      <c r="B17" s="12" t="b">
         <f>IF(_i_cia_interest_asked="",FALSE,_i_cia_interest_asked)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="23" t="b">
+      <c r="B18" s="12" t="b">
         <f>AND(_i_cia_interest_asked,_i_interestRate1&lt;&gt;"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="23" t="b">
+      <c r="B19" s="12" t="b">
         <f>AND(NOT(_t_cia_interest_conflict),_d_dtCalc&gt;=DATE(2020,12,1))</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="23" t="b">
+      <c r="B20" s="12" t="b">
         <f>AND(_t_cia_interest_asked,_cia_interest_available)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="11" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="23" t="b">
+      <c r="B24" s="12" t="b">
         <f>IF(_i_cia_indexation_asked="",FALSE,_i_cia_indexation_asked)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="23" t="b">
+      <c r="B25" s="12" t="b">
         <f>AND(_i_cia_indexation_asked,_i_indexationRate1&lt;&gt;"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="23" t="b">
+      <c r="B26" s="12" t="b">
         <f>AND(NOT(_t_cia_indexation_conflict),_d_dtCalc&gt;=DATE(2020,12,1))</f>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="23" t="b">
+      <c r="B27" s="12" t="b">
         <f>AND(_t_cia_indexation_asked,_cia_indexation_available)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="20" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="32" t="b">
+      <c r="B30" s="21" t="b">
         <f>OR(_e_error1&lt;&gt;"",_e_error2&lt;&gt;"",_e_error3&lt;&gt;"",_e_error4&lt;&gt;"",_e_error5&lt;&gt;"")</f>
         <v>0</v>
       </c>
-      <c r="C30" s="32" t="b">
+      <c r="C30" s="21" t="b">
         <f>AND(_cia_indexation_warning,NOT(OR(_e_error1&lt;&gt;"",_e_error2&lt;&gt;"",_e_error3&lt;&gt;"",_e_error4&lt;&gt;"")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="32" t="b">
+      <c r="B31" s="21" t="b">
         <f>AND(_t_cia_interest_show,_i_indexationRate1&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="32" t="b">
+      <c r="B32" s="21" t="b">
         <f>NOT(OR(_settings_invalid,_e_error1&lt;&gt;"",_e_error2&lt;&gt;"",_e_error3&lt;&gt;"",_e_error4&lt;&gt;""))</f>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="23">
+      <c r="B34" s="12">
         <f>_t_age1+_t_deferred+IF(NOT(_t_due),1/_t_frequency,0)</f>
         <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="12">
         <f>IF(_i_fracFirstIndexation="",1,_i_fracFirstIndexation)</f>
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="23">
+      <c r="B38" s="12">
         <f>IF(_i_sex1&gt;=1,_i_sex1,_d_sex1)</f>
         <v>1</v>
       </c>
-      <c r="C38" s="23">
+      <c r="C38" s="12">
         <f>IF(_i_sex2&gt;=1,_i_sex2,_t_sex2_temp)</f>
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="23" t="str">
+      <c r="B39" s="12" t="str">
         <f>IF(_t_cia_interest_show,"CPM2014",IF(_i_qxTable1="",IF(_s_country="United States","RP2014A","CPM2014"),_i_qxTable1))</f>
-        <v>RP2014A</v>
-      </c>
-      <c r="C39" s="23" t="str">
+        <v>CPM2014</v>
+      </c>
+      <c r="C39" s="12" t="str">
         <f>IF(_t_hasReversion,IF(_t_cia_interest_show,"CPM2014",IF(_i_qxTable2="",IF(_s_country="United States","RP2014A","CPM2014"),_i_qxTable2)),"")</f>
-        <v>RP2014D</v>
+        <v/>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="23" t="b">
+      <c r="B40" s="12" t="b">
         <f>IF(_t_cia_interest_show,TRUE,IF(OR(_i_qxScale1="None",_i_qxScale1=""),FALSE,TRUE))</f>
         <v>0</v>
       </c>
-      <c r="C40" s="23" t="b">
+      <c r="C40" s="12" t="b">
         <f>IF(AND(_t_hasReversion,_t_cia_interest_show),TRUE,IF(OR(_i_qxScale2="None",_i_qxScale2=""),FALSE,TRUE))</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="40" t="str">
+      <c r="B41" s="29" t="str">
         <f>IF(_t_cia_interest_show,"ECH_CPM_B",IF(OR(_i_qxScale1="None",_i_qxScale1=""),"",_i_qxScale1))</f>
         <v/>
       </c>
-      <c r="C41" s="40" t="str">
+      <c r="C41" s="29" t="str">
         <f>IF(AND(_t_hasReversion,_t_cia_interest_show),"ECH_CPM_B",IF(OR(_i_qxScale2="None",_i_qxScale2=""),"",_i_qxScale2))</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="23">
+      <c r="B42" s="12">
         <f>IF(_t_cia_interest_show,YEAR(_d_dtCalc),IF(_i_qxValuationYear1&gt;0,_i_qxValuationYear1,IF(_d_dtCalc&gt;0,YEAR(_d_dtCalc),YEAR(_t_today))))</f>
         <v>2021</v>
       </c>
-      <c r="C42" s="23">
+      <c r="C42" s="12">
         <f>IF(_t_cia_interest_show,YEAR(_d_dtCalc),IF(_i_qxValuationYear2&gt;0,_i_qxValuationYear2,IF(_d_dtCalc&gt;0,YEAR(_d_dtCalc),YEAR(_t_today))))</f>
         <v>2021</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="23">
+      <c r="B43" s="12">
         <f>IF(_ic_qxAgeValuation1="",0,_ic_qxAgeValuation1)</f>
         <v>0</v>
       </c>
-      <c r="C43" s="23">
+      <c r="C43" s="12">
         <f>IF(_ic_qxAgeValuation2="",0,_ic_qxAgeValuation2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="B44" s="23" t="str">
+      <c r="A44" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="12" t="str">
         <f>VLOOKUP(_t_qxTable1,_z_tabQxTable,3,FALSE)</f>
-        <v>RP-2014 Rates-Healthy annuitant</v>
-      </c>
-      <c r="C44" s="23" t="str">
+        <v>Canadian Pensioners’ Mortality (CPM) 2014, composite of Public and Private Sector</v>
+      </c>
+      <c r="C44" s="12" t="str">
         <f>IF(_t_qxTable2="","",VLOOKUP(_t_qxTable2,_z_tabQxTable,3,FALSE))</f>
-        <v>RP-2014 Rates-Disabled annuitant</v>
+        <v/>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C45" s="23"/>
+      <c r="C45" s="12"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="23">
+      <c r="B47" s="12">
         <f>IF(_i_guarantee="",0,_i_guarantee)</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="23">
+      <c r="B48" s="12">
         <f>IF(_i_reversion="",0,_i_reversion)</f>
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="34" t="s">
+      <c r="A49" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="23">
+      <c r="B49" s="12">
         <f>IF(_i_deferred="",0,_i_deferred)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="23">
+      <c r="B50" s="12">
         <f>IF(_i_frequency="",12,_i_frequency)</f>
         <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B51" s="23" t="b">
+      <c r="B51" s="12" t="b">
         <f>IF(_i_due="",TRUE,_i_due)</f>
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="34" t="s">
+      <c r="A52" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="23" t="b">
+      <c r="B52" s="12" t="b">
         <f>IF(_i_qxPre="",TRUE,_i_qxPre)</f>
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E54" s="36"/>
+      <c r="E54" s="25"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B55" s="26">
+      <c r="B55" s="15">
         <f ca="1">TODAY()</f>
-        <v>44511</v>
-      </c>
-      <c r="E55" s="36"/>
+        <v>44512</v>
+      </c>
+      <c r="E55" s="25"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B56" s="68" cm="1">
+      <c r="B56" s="50" cm="1">
         <f t="array" ref="B56">IF(_d_dtCalc&lt;&gt;0,_xll.FirstDayOfMonth(_d_dtCalc,FALSE),_xll.FirstDayOfMonth("_t_today",FALSE))</f>
         <v>44501</v>
       </c>
-      <c r="E56" s="36"/>
+      <c r="E56" s="25"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B57" s="68" cm="1">
+      <c r="B57" s="50" cm="1">
         <f t="array" aca="1" ref="B57" ca="1">[1]!_lastDateCIAStat</f>
         <v>44501</v>
       </c>
-      <c r="E57" s="36"/>
+      <c r="E57" s="25"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="22" t="s">
+      <c r="A58" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="68">
+      <c r="B58" s="50">
         <f ca="1">IF(_d_dtCalc&gt;0,MIN(_d_dtCalc,_t_today,date_cia_latest),MIN(_t_today,date_cia_latest))</f>
         <v>44501</v>
       </c>
-      <c r="E58" s="36"/>
+      <c r="E58" s="25"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B59" s="45">
+      <c r="B59" s="34">
         <f>_i_indexation_offset</f>
         <v>0</v>
       </c>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B60" s="45">
+      <c r="B60" s="34">
         <f>IF(_i_indexation_fraction="",1,_i_indexation_fraction)</f>
         <v>1</v>
       </c>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="22" t="s">
+      <c r="A61" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="45">
+      <c r="B61" s="34">
         <f>IF(_i_indexation_max="",1000,_i_indexation_max)</f>
         <v>1000</v>
       </c>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="27" t="s">
+      <c r="A62" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B62" s="116" t="b">
+      <c r="B62" s="98" t="b">
         <f ca="1">B56&lt;&gt;date_cia_latest</f>
         <v>0</v>
       </c>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-    </row>
-    <row r="63" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="34"/>
-      <c r="B63" s="35">
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+    </row>
+    <row r="63" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="23"/>
+      <c r="B63" s="24">
         <v>36</v>
       </c>
-      <c r="C63" s="36">
+      <c r="C63" s="25">
         <v>5</v>
       </c>
-      <c r="D63" s="36">
+      <c r="D63" s="25">
         <v>37</v>
       </c>
-      <c r="E63" s="63"/>
+      <c r="E63" s="46"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B64" s="37" cm="1">
+      <c r="B64" s="26" cm="1">
         <f t="array" aca="1" ref="B64" ca="1">_xll.CIA(_t_dtCIA,B63)</f>
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C64" s="23" cm="1">
+      <c r="C64" s="12" cm="1">
         <f t="array" aca="1" ref="C64" ca="1">_xll.CIA(_t_dtCIA,C63)</f>
         <v>10</v>
       </c>
-      <c r="D64" s="37" cm="1">
+      <c r="D64" s="26" cm="1">
         <f t="array" aca="1" ref="D64" ca="1">_xll.CIA(_t_dtCIA,D63)</f>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="E64" s="37"/>
+      <c r="E64" s="26"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B65" s="38" cm="1">
+      <c r="B65" s="27" cm="1">
         <f t="array" aca="1" ref="B65" ca="1">_xll.CIA(_t_dtCIA,B67)</f>
         <v>1.4055899900391022E-2</v>
       </c>
-      <c r="C65" s="23"/>
-      <c r="D65" s="38" cm="1">
+      <c r="C65" s="12"/>
+      <c r="D65" s="27" cm="1">
         <f t="array" aca="1" ref="D65" ca="1">_xll.CIA(_t_dtCIA,D67)</f>
         <v>2.0534488581689381E-2</v>
       </c>
-      <c r="E65" s="37"/>
-      <c r="F65" s="46"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="35"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B66" s="38">
+      <c r="B66" s="27">
         <f ca="1">MAX(0,MIN(_t_indexation_max,(B65-_i_indexation_offset)*_t_indexation_fraction))</f>
         <v>1.4055899900391022E-2</v>
       </c>
-      <c r="C66" s="23">
+      <c r="C66" s="12">
         <f ca="1">C64</f>
         <v>10</v>
       </c>
-      <c r="D66" s="38">
+      <c r="D66" s="27">
         <f ca="1">MAX(0,MIN(_t_indexation_max,(D65-_i_indexation_offset)*_t_indexation_fraction))</f>
         <v>2.0534488581689381E-2</v>
       </c>
-      <c r="E66" s="38"/>
+      <c r="E66" s="27"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B67" s="35">
+      <c r="B67" s="24">
         <v>38</v>
       </c>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36">
+      <c r="C67" s="25"/>
+      <c r="D67" s="25">
         <v>39</v>
       </c>
-      <c r="E67" s="36"/>
+      <c r="E67" s="25"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="39"/>
-      <c r="B68" s="40"/>
-      <c r="C68" s="145" t="s">
+      <c r="A68" s="28"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D68" s="145"/>
-      <c r="E68" s="145"/>
+      <c r="D68" s="142"/>
+      <c r="E68" s="142"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="39"/>
-      <c r="B69" s="40"/>
-      <c r="C69" s="41" t="s">
+      <c r="A69" s="28"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="D69" s="41" t="s">
+      <c r="D69" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="E69" s="41" t="s">
+      <c r="E69" s="30" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="39" t="s">
+      <c r="A70" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="40" t="s">
+      <c r="B70" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C70" s="42" t="b">
+      <c r="C70" s="31" t="b">
         <f>OR(_i_qxTable1="",_i_qxTable1=_cia_table)</f>
-        <v>0</v>
-      </c>
-      <c r="D70" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70" s="31" t="b">
         <f>OR(_i_qxTable2="",_i_qxTable2=_cia_table)</f>
-        <v>0</v>
-      </c>
-      <c r="E70" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="31" t="b">
         <f>AND(C70:D70)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="39" t="s">
+      <c r="A71" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B71" s="40" t="s">
+      <c r="B71" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C71" s="42" t="b">
+      <c r="C71" s="31" t="b">
         <f>OR(_i_qxScale1="",_i_qxScale1=_cia_scale)</f>
         <v>1</v>
       </c>
-      <c r="D71" s="42" t="b">
+      <c r="D71" s="31" t="b">
         <f>OR(_i_qxScale2="",_i_qxScale2=_cia_scale)</f>
         <v>1</v>
       </c>
-      <c r="E71" s="42" t="b">
+      <c r="E71" s="31" t="b">
         <f t="shared" ref="E71:E73" si="0">AND(C71:D71)</f>
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="39" t="s">
+      <c r="A72" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B72" s="40">
+      <c r="B72" s="29">
         <v>0</v>
       </c>
-      <c r="C72" s="42" t="b">
+      <c r="C72" s="31" t="b">
         <f>OR(_i_qxShitAge1=0,_i_qxShitAge1=_cia_shift_age)</f>
         <v>1</v>
       </c>
-      <c r="D72" s="42" t="b">
+      <c r="D72" s="31" t="b">
         <f>OR(_i_qxShitAge2=0,_i_qxShitAge2=_cia_shift_age)</f>
         <v>1</v>
       </c>
-      <c r="E72" s="42" t="b">
+      <c r="E72" s="31" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="39" t="s">
+      <c r="A73" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B73" s="40">
+      <c r="B73" s="29">
         <v>0</v>
       </c>
-      <c r="C73" s="42" t="b">
+      <c r="C73" s="31" t="b">
         <f>OR(_i_qxLoading1=0,_i_qxLoading1=_cia_loading)</f>
         <v>1</v>
       </c>
-      <c r="D73" s="42" t="b">
+      <c r="D73" s="31" t="b">
         <f>OR(_i_qxLoading2=0,_i_qxLoading2=_cia_loading)</f>
         <v>1</v>
       </c>
-      <c r="E73" s="42" t="b">
+      <c r="E73" s="31" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B74" s="40">
+      <c r="B74" s="29">
         <f>YEAR(_d_dtCalc)</f>
         <v>2021</v>
       </c>
-      <c r="C74" s="42" t="b">
+      <c r="C74" s="31" t="b">
         <f>OR(_i_qxValuationYear1="",_i_qxValuationYear1=_cia_year)</f>
         <v>1</v>
       </c>
-      <c r="D74" s="42" t="b">
+      <c r="D74" s="31" t="b">
         <f>OR(_i_qxValuationYear2="",_i_qxValuationYear2=_cia_year)</f>
         <v>1</v>
       </c>
-      <c r="E74" s="42" t="b">
+      <c r="E74" s="31" t="b">
         <f>AND(C74:D74)</f>
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="39" t="s">
+      <c r="A75" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="B75" s="40"/>
-      <c r="C75" s="42"/>
-      <c r="D75" s="42"/>
-      <c r="E75" s="42" t="b">
+      <c r="B75" s="29"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31" t="b">
         <f>OR(NOT(_t_cia_interest_show),AND(E70:E74))</f>
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" s="22" t="s">
+      <c r="A77" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B77" s="45">
+      <c r="B77" s="34">
         <f>IF(_i_indexationRate1="",0,_i_indexationRate1)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="zc5d17GuMCXa+gU6zxac99VsA3P2h9f0g/w5+qGmoTAieAkvFYVlrFY283/3FcT34hWz1Z2xZWEbpVyOJyrX1w==" saltValue="HVqxEmumvqtHeZlLLUC7+A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="C68:E68"/>
   </mergeCells>

</xml_diff>